<commit_message>
[docs-only] Update the added services per release table
</commit_message>
<xml_diff>
--- a/docs/services/general-info/added-services.xlsx
+++ b/docs/services/general-info/added-services.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\ownCloud\diemattels.at\martin@filer\Dokumente\Firma\Kunden\ownCloud\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\ownCloud\diemattels.at\dev image share\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E2217C8-838F-4AA0-B35C-5A6558345497}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A430EAF4-9B3E-4933-A96E-20DFA8D22A50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="490" yWindow="100" windowWidth="17070" windowHeight="9680" xr2:uid="{39CF58C5-54CC-4925-B484-35B2EEB23194}"/>
+    <workbookView xWindow="1870" yWindow="490" windowWidth="17070" windowHeight="9680" xr2:uid="{39CF58C5-54CC-4925-B484-35B2EEB23194}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="48">
   <si>
     <t>4.0</t>
   </si>
@@ -177,6 +177,9 @@
   </si>
   <si>
     <t>7.0</t>
+  </si>
+  <si>
+    <t>auth-app</t>
   </si>
 </sst>
 </file>
@@ -559,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CE9FA73-9F35-485D-9DC1-6178D0D26E91}">
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -664,598 +667,603 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" t="s">
-        <v>8</v>
-      </c>
       <c r="E7" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>11</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>12</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D11" t="s">
         <v>12</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="C11" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C12" t="s">
         <v>13</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D12" t="s">
         <v>13</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="D12" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D13" t="s">
         <v>14</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E13" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="C13" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C14" t="s">
         <v>11</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D14" t="s">
         <v>11</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E14" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" t="s">
+        <v>23</v>
+      </c>
+      <c r="E23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
         <v>24</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>24</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
         <v>24</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D24" t="s">
         <v>24</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E24" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="C24" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C25" t="s">
         <v>25</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D25" t="s">
         <v>25</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E25" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25" t="s">
-        <v>26</v>
-      </c>
-      <c r="D25" t="s">
-        <v>26</v>
-      </c>
-      <c r="E25" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" t="s">
+        <v>31</v>
+      </c>
+      <c r="D31" t="s">
+        <v>31</v>
+      </c>
+      <c r="E31" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
         <v>32</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>32</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C32" t="s">
         <v>32</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D32" t="s">
         <v>32</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E32" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="C32" t="s">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C33" t="s">
         <v>33</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D33" t="s">
         <v>33</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E33" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>34</v>
-      </c>
-      <c r="B33" t="s">
-        <v>34</v>
-      </c>
-      <c r="C33" t="s">
-        <v>34</v>
-      </c>
-      <c r="D33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E33" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B34" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C34" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D34" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E34" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C36" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D36" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E36" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C37" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D37" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E37" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C38" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D38" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E38" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C39" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D39" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E39" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C40" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D40" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E40" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C42" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D42" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E42" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
+        <v>43</v>
+      </c>
+      <c r="B43" t="s">
+        <v>43</v>
+      </c>
+      <c r="C43" t="s">
+        <v>43</v>
+      </c>
+      <c r="D43" t="s">
+        <v>43</v>
+      </c>
+      <c r="E43" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
         <v>44</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>44</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C44" t="s">
         <v>44</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D44" t="s">
         <v>44</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E44" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>